<commit_message>
removing unnecessary files and renaming files
</commit_message>
<xml_diff>
--- a/emails_muq.xlsx
+++ b/emails_muq.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar.singh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumar.singh\Desktop\sharepoint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="23055" windowHeight="9945"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="23055" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="emails_muq" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>Subgroup name</t>
   </si>
@@ -142,13 +142,16 @@
   </si>
   <si>
     <t>Retail</t>
+  </si>
+  <si>
+    <t>cs.satish@mu-sigma.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +282,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -581,7 +592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -624,11 +635,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -662,6 +675,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -951,12 +965,13 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -974,18 +989,18 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
@@ -1334,6 +1349,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
collate file added, too much struggle to remove hexadecimals, fianlly done
</commit_message>
<xml_diff>
--- a/emails_muq.xlsx
+++ b/emails_muq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="23055" windowHeight="9945"/>
+    <workbookView xWindow="7560" yWindow="0" windowWidth="23055" windowHeight="9945"/>
   </bookViews>
   <sheets>
     <sheet name="emails_muq" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Subgroup name</t>
   </si>
@@ -30,121 +30,28 @@
     <t>Team members</t>
   </si>
   <si>
+    <t>ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com</t>
+  </si>
+  <si>
+    <t>anantdeep.parihar@mu-sigma.com</t>
+  </si>
+  <si>
+    <t>ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com</t>
+  </si>
+  <si>
+    <t>Marketing - Agile</t>
+  </si>
+  <si>
+    <t>Marketing - Consumer</t>
+  </si>
+  <si>
+    <t>Marketing - Customer Insights</t>
+  </si>
+  <si>
     <t>kumar.singh@mu-sigma.com</t>
   </si>
   <si>
-    <t>ashish.sorout@mu-sigma.com</t>
-  </si>
-  <si>
-    <t>ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com</t>
-  </si>
-  <si>
-    <t>anantdeep.parihar@mu-sigma.com</t>
-  </si>
-  <si>
-    <t>ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com; ashish.sorout@mu-sigma.com</t>
-  </si>
-  <si>
-    <t>Marketing - Agile</t>
-  </si>
-  <si>
-    <t>Marketing - Consumer</t>
-  </si>
-  <si>
-    <t>Marketing - Customer Insights</t>
-  </si>
-  <si>
-    <t>Marketing - MS&amp;A</t>
-  </si>
-  <si>
-    <t>Marketing – PRO</t>
-  </si>
-  <si>
-    <t>FP&amp;A – RI</t>
-  </si>
-  <si>
-    <t>FP&amp;A - Forecasting</t>
-  </si>
-  <si>
-    <t>FP&amp;A - Lift + GM</t>
-  </si>
-  <si>
-    <t>FP&amp;A - Store Planning</t>
-  </si>
-  <si>
-    <t>Canada – Store Ops</t>
-  </si>
-  <si>
-    <t>Canada – Building services</t>
-  </si>
-  <si>
-    <t>Merchandising - Pricing</t>
-  </si>
-  <si>
-    <t>Merchandising – Pro Pricing</t>
-  </si>
-  <si>
-    <t>Merchandising - Black Locus – VPP</t>
-  </si>
-  <si>
-    <t>Merchandising - AP 1.0</t>
-  </si>
-  <si>
-    <t>Merchandising - AP 2.0</t>
-  </si>
-  <si>
-    <t>Credit Services</t>
-  </si>
-  <si>
-    <t>RPV</t>
-  </si>
-  <si>
-    <t>S&amp;PS</t>
-  </si>
-  <si>
-    <t>GE – Appliances</t>
-  </si>
-  <si>
-    <t>CCNA</t>
-  </si>
-  <si>
-    <t>CCRC</t>
-  </si>
-  <si>
-    <t>ARA</t>
-  </si>
-  <si>
-    <t>Decision Sciences </t>
-  </si>
-  <si>
-    <t>Data Science</t>
-  </si>
-  <si>
-    <t>DTC RI</t>
-  </si>
-  <si>
-    <t>NFS</t>
-  </si>
-  <si>
-    <t>SCM</t>
-  </si>
-  <si>
-    <t>ESI</t>
-  </si>
-  <si>
-    <t>PSP</t>
-  </si>
-  <si>
-    <t>Payer Mix</t>
-  </si>
-  <si>
-    <t>WWS</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>cs.satish@mu-sigma.com</t>
+    <t>c.satish@mu-sigma.com</t>
   </si>
 </sst>
 </file>
@@ -962,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,372 +894,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>